<commit_message>
Update upload work sample and extent reports
</commit_message>
<xml_diff>
--- a/marsframework/marsframework-master/Mars.xlsx
+++ b/marsframework/marsframework-master/Mars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="10740" tabRatio="779" activeTab="3"/>
+    <workbookView windowWidth="17440" windowHeight="8370" tabRatio="779" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Conditions-Share Skill" sheetId="1" r:id="rId1"/>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>2.</t>
     </r>
     <r>
@@ -1070,7 +1076,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1105,10 +1111,49 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1120,15 +1165,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1142,9 +1209,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1159,14 +1242,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1176,83 +1252,6 @@
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1271,7 +1270,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1283,7 +1324,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1295,25 +1378,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1331,127 +1444,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1480,6 +1479,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1495,13 +1503,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1523,24 +1535,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1563,8 +1562,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1582,152 +1581,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1749,29 +1748,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2134,23 +2115,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="22.9090909090909" style="10" customWidth="1"/>
-    <col min="2" max="2" width="27.7272727272727" style="10" customWidth="1"/>
-    <col min="3" max="3" width="44.7272727272727" style="7" customWidth="1"/>
-    <col min="4" max="4" width="53.3636363636364" style="7" customWidth="1"/>
+    <col min="1" max="1" width="22.9090909090909" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.7272727272727" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.7272727272727" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.3636363636364" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2169,380 +2150,380 @@
       </c>
     </row>
     <row r="4" ht="28" spans="1:4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="28" spans="4:4">
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" ht="28" spans="4:4">
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" ht="28" spans="1:4">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="28" spans="4:4">
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" ht="28" spans="4:4">
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" ht="28" spans="1:4">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" ht="28" spans="4:4">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" ht="28" spans="4:4">
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" ht="28" spans="4:4">
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" ht="28" spans="1:4">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" ht="28" spans="4:4">
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" ht="28" spans="4:4">
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" ht="28" spans="1:4">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" ht="28" spans="4:4">
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" ht="28" spans="1:4">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" ht="28" spans="4:4">
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" ht="28" spans="1:4">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" ht="28" spans="4:4">
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" ht="28" spans="4:4">
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" ht="28" spans="4:4">
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" ht="28" spans="4:4">
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="32" ht="28" spans="4:4">
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" ht="28" spans="4:4">
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="34" ht="28" spans="4:4">
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" ht="28" spans="4:4">
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" ht="28" spans="4:4">
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="37" ht="28" spans="4:4">
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" ht="28" spans="4:4">
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" ht="28" spans="4:4">
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40" ht="28" spans="4:4">
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="41" ht="28" spans="4:4">
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="42" ht="28" spans="4:4">
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="43" ht="28" spans="4:4">
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="44" ht="28" spans="4:4">
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="45" ht="28" spans="4:4">
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="46" ht="28" spans="4:4">
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="48" ht="28" spans="1:4">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="49" ht="28" spans="4:4">
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" ht="28" spans="4:4">
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="51" ht="28" spans="4:4">
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="52" ht="28" spans="4:4">
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="53" ht="28" spans="4:4">
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="54" ht="28" spans="4:4">
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="55" ht="28" spans="4:4">
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="56" ht="28" spans="4:4">
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="57" ht="28" spans="4:4">
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" ht="28" spans="1:4">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="60" ht="28" spans="4:4">
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="61" ht="28" spans="4:4">
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" ht="28" spans="1:4">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="64" ht="28" spans="4:4">
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="66" ht="28" spans="1:4">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="68" ht="28" spans="1:4">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2558,22 +2539,22 @@
   <sheetPr/>
   <dimension ref="A1:H379"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F309" sqref="F309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="16.4545454545455" style="11" customWidth="1"/>
-    <col min="2" max="2" width="25.3636363636364" style="12" customWidth="1"/>
-    <col min="3" max="3" width="42.0909090909091" style="12" customWidth="1"/>
-    <col min="4" max="4" width="41.7272727272727" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.6363636363636" style="12" customWidth="1"/>
-    <col min="6" max="6" width="14.2727272727273" style="12" customWidth="1"/>
-    <col min="7" max="7" width="15.0909090909091" style="12" customWidth="1"/>
-    <col min="8" max="8" width="15.6363636363636" style="12" customWidth="1"/>
+    <col min="1" max="1" width="16.4545454545455" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.3636363636364" style="9" customWidth="1"/>
+    <col min="3" max="3" width="42.0909090909091" style="9" customWidth="1"/>
+    <col min="4" max="4" width="41.7272727272727" style="9" customWidth="1"/>
+    <col min="5" max="5" width="17.6363636363636" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.2727272727273" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.0909090909091" style="9" customWidth="1"/>
+    <col min="8" max="8" width="15.6363636363636" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.75" spans="1:8">
@@ -2603,10 +2584,10 @@
       </c>
     </row>
     <row r="2" ht="28" spans="1:4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -2617,8 +2598,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="5" t="s">
         <v>97</v>
       </c>
@@ -2627,8 +2608,8 @@
       </c>
     </row>
     <row r="4" ht="42" spans="1:4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="5" t="s">
         <v>99</v>
       </c>
@@ -2637,8 +2618,8 @@
       </c>
     </row>
     <row r="5" ht="28" spans="1:4">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="5" t="s">
         <v>101</v>
       </c>
@@ -2647,16 +2628,16 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" ht="28" spans="1:4">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2666,9 +2647,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
+    <row r="8" spans="2:4">
+      <c r="B8" s="4"/>
       <c r="C8" s="5" t="s">
         <v>97</v>
       </c>
@@ -2676,9 +2656,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" ht="42" spans="1:4">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
+    <row r="9" ht="42" spans="2:4">
+      <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>99</v>
       </c>
@@ -2686,9 +2665,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" ht="28" spans="1:4">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+    <row r="10" ht="28" spans="2:4">
+      <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
         <v>101</v>
       </c>
@@ -2696,34 +2674,29 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" ht="28" spans="1:4">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+    <row r="11" ht="28" spans="2:4">
+      <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12" t="s">
+    <row r="12" spans="2:4">
+      <c r="B12" s="4"/>
+      <c r="C12" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="14"/>
-    </row>
     <row r="14" ht="28" spans="1:4">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -2734,8 +2707,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="9"/>
       <c r="C15" s="5" t="s">
         <v>97</v>
       </c>
@@ -2744,8 +2716,7 @@
       </c>
     </row>
     <row r="16" ht="42" spans="1:4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="9"/>
       <c r="C16" s="5" t="s">
         <v>99</v>
       </c>
@@ -2754,8 +2725,7 @@
       </c>
     </row>
     <row r="17" ht="28" spans="1:4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="9"/>
       <c r="C17" s="5" t="s">
         <v>101</v>
       </c>
@@ -2764,30 +2734,28 @@
       </c>
     </row>
     <row r="18" ht="28" spans="1:4">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="9"/>
       <c r="C18" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
+      <c r="A19" s="9"/>
+      <c r="C19" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" ht="28" spans="1:4">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -2798,8 +2766,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="15"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="9"/>
       <c r="C22" s="5" t="s">
         <v>97</v>
       </c>
@@ -2808,8 +2775,7 @@
       </c>
     </row>
     <row r="23" ht="42" spans="1:4">
-      <c r="A23" s="15"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="9"/>
       <c r="C23" s="5" t="s">
         <v>99</v>
       </c>
@@ -2818,8 +2784,7 @@
       </c>
     </row>
     <row r="24" ht="28" spans="1:4">
-      <c r="A24" s="15"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="9"/>
       <c r="C24" s="5" t="s">
         <v>101</v>
       </c>
@@ -2828,30 +2793,28 @@
       </c>
     </row>
     <row r="25" ht="28" spans="1:4">
-      <c r="A25" s="15"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="9"/>
       <c r="C25" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="15"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12" t="s">
+      <c r="A26" s="9"/>
+      <c r="C26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="28" ht="42" spans="1:4">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -2889,23 +2852,23 @@
       <c r="C32" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="9" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="33" ht="28" spans="3:4">
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="9" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="35" ht="42" spans="1:4">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -2915,7 +2878,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" ht="42" spans="3:4">
+    <row r="36" spans="3:4">
       <c r="C36" s="5" t="s">
         <v>97</v>
       </c>
@@ -2943,23 +2906,23 @@
       <c r="C39" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="40" spans="3:4">
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="6" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="42" ht="42" spans="1:4">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -2997,23 +2960,23 @@
       <c r="C46" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="9" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="47" ht="28" spans="3:4">
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="9" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="49" ht="42" spans="1:4">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -3048,26 +3011,26 @@
       </c>
     </row>
     <row r="53" spans="3:4">
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="54" spans="3:4">
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="56" ht="42" spans="1:4">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -3102,26 +3065,26 @@
       </c>
     </row>
     <row r="60" spans="3:4">
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="61" spans="3:4">
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="9" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="63" ht="42" spans="1:4">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -3156,42 +3119,42 @@
       </c>
     </row>
     <row r="67" spans="3:4">
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="68" spans="3:4">
-      <c r="C68" s="12" t="s">
+      <c r="C68" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="69" ht="28" spans="3:4">
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="9" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="70" ht="28" spans="3:4">
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="9" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="72" ht="42" spans="1:4">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -3226,42 +3189,42 @@
       </c>
     </row>
     <row r="76" spans="3:4">
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D76" s="12" t="s">
+      <c r="D76" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="77" spans="3:4">
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="9" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="78" ht="28" spans="3:4">
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="9" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="79" ht="28" spans="3:4">
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="9" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="81" ht="42" spans="1:4">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C81" s="5" t="s">
@@ -3296,26 +3259,26 @@
       </c>
     </row>
     <row r="85" ht="28" spans="3:4">
-      <c r="C85" s="12" t="s">
+      <c r="C85" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="9" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="86" spans="3:4">
-      <c r="C86" s="12" t="s">
+      <c r="C86" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="9" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="88" ht="42" spans="1:4">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C88" s="5" t="s">
@@ -3350,34 +3313,34 @@
       </c>
     </row>
     <row r="92" ht="28" spans="3:4">
-      <c r="C92" s="12" t="s">
+      <c r="C92" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D92" s="9" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="93" spans="3:4">
-      <c r="C93" s="12" t="s">
+      <c r="C93" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="9" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="94" ht="28" spans="3:4">
-      <c r="C94" s="12" t="s">
+      <c r="C94" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D94" s="12" t="s">
+      <c r="D94" s="9" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="96" ht="42" spans="1:4">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B96" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C96" s="5" t="s">
@@ -3412,18 +3375,18 @@
       </c>
     </row>
     <row r="100" spans="3:4">
-      <c r="C100" s="12" t="s">
+      <c r="C100" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="9" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="102" ht="56" spans="1:4">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C102" s="5" t="s">
@@ -3458,18 +3421,18 @@
       </c>
     </row>
     <row r="106" ht="42" spans="3:4">
-      <c r="C106" s="12" t="s">
+      <c r="C106" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D106" s="12" t="s">
+      <c r="D106" s="9" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="108" ht="56" spans="1:4">
-      <c r="A108" s="10" t="s">
+      <c r="A108" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B108" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C108" s="5" t="s">
@@ -3504,18 +3467,18 @@
       </c>
     </row>
     <row r="112" ht="28" spans="3:4">
-      <c r="C112" s="12" t="s">
+      <c r="C112" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="D112" s="12" t="s">
+      <c r="D112" s="9" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="114" ht="42" spans="1:4">
-      <c r="A114" s="10" t="s">
+      <c r="A114" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B114" s="7" t="s">
+      <c r="B114" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C114" s="5" t="s">
@@ -3550,18 +3513,18 @@
       </c>
     </row>
     <row r="118" ht="28" spans="3:4">
-      <c r="C118" s="12" t="s">
+      <c r="C118" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D118" s="12" t="s">
+      <c r="D118" s="9" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="120" ht="42" spans="1:4">
-      <c r="A120" s="10" t="s">
+      <c r="A120" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B120" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C120" s="5" t="s">
@@ -3596,18 +3559,18 @@
       </c>
     </row>
     <row r="124" ht="28" spans="3:4">
-      <c r="C124" s="12" t="s">
+      <c r="C124" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D124" s="12" t="s">
+      <c r="D124" s="9" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="126" ht="42" spans="1:4">
-      <c r="A126" s="10" t="s">
+      <c r="A126" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="B126" s="4" t="s">
         <v>170</v>
       </c>
       <c r="C126" s="5" t="s">
@@ -3642,26 +3605,26 @@
       </c>
     </row>
     <row r="130" ht="28" spans="3:4">
-      <c r="C130" s="12" t="s">
+      <c r="C130" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D130" s="12" t="s">
+      <c r="D130" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="131" spans="3:4">
-      <c r="C131" s="12" t="s">
+      <c r="C131" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D131" s="12" t="s">
+      <c r="D131" s="9" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="133" ht="56" spans="1:4">
-      <c r="A133" s="10" t="s">
+      <c r="A133" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B133" s="7" t="s">
+      <c r="B133" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C133" s="5" t="s">
@@ -3696,26 +3659,26 @@
       </c>
     </row>
     <row r="137" ht="28" spans="3:4">
-      <c r="C137" s="12" t="s">
+      <c r="C137" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D137" s="12" t="s">
+      <c r="D137" s="9" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="138" ht="28" spans="3:4">
-      <c r="C138" s="12" t="s">
+      <c r="C138" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D138" s="12" t="s">
+      <c r="D138" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="140" ht="56" spans="1:4">
-      <c r="A140" s="10" t="s">
+      <c r="A140" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B140" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C140" s="5" t="s">
@@ -3750,26 +3713,26 @@
       </c>
     </row>
     <row r="144" ht="28" spans="3:4">
-      <c r="C144" s="12" t="s">
+      <c r="C144" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D144" s="12" t="s">
+      <c r="D144" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="145" spans="3:4">
-      <c r="C145" s="12" t="s">
+      <c r="C145" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D145" s="12" t="s">
+      <c r="D145" s="9" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="147" ht="56" spans="1:4">
-      <c r="A147" s="10" t="s">
+      <c r="A147" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B147" s="7" t="s">
+      <c r="B147" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C147" s="5" t="s">
@@ -3804,26 +3767,26 @@
       </c>
     </row>
     <row r="151" ht="28" spans="3:4">
-      <c r="C151" s="12" t="s">
+      <c r="C151" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D151" s="12" t="s">
+      <c r="D151" s="9" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="152" ht="28" spans="3:4">
-      <c r="C152" s="12" t="s">
+      <c r="C152" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D152" s="12" t="s">
+      <c r="D152" s="9" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="154" ht="42" spans="1:4">
-      <c r="A154" s="10" t="s">
+      <c r="A154" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B154" s="7" t="s">
+      <c r="B154" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C154" s="5" t="s">
@@ -3858,26 +3821,26 @@
       </c>
     </row>
     <row r="158" ht="28" spans="3:4">
-      <c r="C158" s="12" t="s">
+      <c r="C158" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="D158" s="12" t="s">
+      <c r="D158" s="9" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="159" spans="3:4">
-      <c r="C159" s="12" t="s">
+      <c r="C159" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D159" s="12" t="s">
+      <c r="D159" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="161" ht="42" spans="1:4">
-      <c r="A161" s="10" t="s">
+      <c r="A161" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B161" s="7" t="s">
+      <c r="B161" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C161" s="5" t="s">
@@ -3912,26 +3875,26 @@
       </c>
     </row>
     <row r="165" ht="28" spans="3:4">
-      <c r="C165" s="12" t="s">
+      <c r="C165" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D165" s="12" t="s">
+      <c r="D165" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="166" spans="3:4">
-      <c r="C166" s="12" t="s">
+      <c r="C166" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D166" s="12" t="s">
+      <c r="D166" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="168" ht="56" spans="1:4">
-      <c r="A168" s="10" t="s">
+      <c r="A168" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B168" s="7" t="s">
+      <c r="B168" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C168" s="5" t="s">
@@ -3966,26 +3929,26 @@
       </c>
     </row>
     <row r="172" ht="28" spans="3:4">
-      <c r="C172" s="12" t="s">
+      <c r="C172" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D172" s="12" t="s">
+      <c r="D172" s="9" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="173" ht="28" spans="3:4">
-      <c r="C173" s="12" t="s">
+      <c r="C173" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D173" s="12" t="s">
+      <c r="D173" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="175" ht="42" spans="1:4">
-      <c r="A175" s="10" t="s">
+      <c r="A175" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B175" s="7" t="s">
+      <c r="B175" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C175" s="5" t="s">
@@ -4020,26 +3983,26 @@
       </c>
     </row>
     <row r="179" ht="28" spans="3:4">
-      <c r="C179" s="12" t="s">
+      <c r="C179" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D179" s="12" t="s">
+      <c r="D179" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="180" spans="3:4">
-      <c r="C180" s="12" t="s">
+      <c r="C180" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D180" s="12" t="s">
+      <c r="D180" s="9" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="182" ht="56" spans="1:4">
-      <c r="A182" s="10" t="s">
+      <c r="A182" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B182" s="7" t="s">
+      <c r="B182" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C182" s="5" t="s">
@@ -4074,26 +4037,26 @@
       </c>
     </row>
     <row r="186" ht="28" spans="3:4">
-      <c r="C186" s="12" t="s">
+      <c r="C186" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D186" s="12" t="s">
+      <c r="D186" s="9" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="187" ht="28" spans="3:4">
-      <c r="C187" s="12" t="s">
+      <c r="C187" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="D187" s="12" t="s">
+      <c r="D187" s="9" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="189" ht="42" spans="1:4">
-      <c r="A189" s="10" t="s">
+      <c r="A189" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B189" s="7" t="s">
+      <c r="B189" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C189" s="5" t="s">
@@ -4128,26 +4091,26 @@
       </c>
     </row>
     <row r="193" ht="28" spans="3:4">
-      <c r="C193" s="12" t="s">
+      <c r="C193" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D193" s="12" t="s">
+      <c r="D193" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="194" spans="3:4">
-      <c r="C194" s="12" t="s">
+      <c r="C194" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D194" s="12" t="s">
+      <c r="D194" s="9" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="196" ht="42" spans="1:4">
-      <c r="A196" s="10" t="s">
+      <c r="A196" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B196" s="7" t="s">
+      <c r="B196" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C196" s="5" t="s">
@@ -4182,26 +4145,26 @@
       </c>
     </row>
     <row r="200" ht="28" spans="3:4">
-      <c r="C200" s="12" t="s">
+      <c r="C200" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D200" s="12" t="s">
+      <c r="D200" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="201" spans="3:4">
-      <c r="C201" s="12" t="s">
+      <c r="C201" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="D201" s="12" t="s">
+      <c r="D201" s="9" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="203" ht="56" spans="1:4">
-      <c r="A203" s="10" t="s">
+      <c r="A203" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="B203" s="7" t="s">
+      <c r="B203" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C203" s="5" t="s">
@@ -4236,26 +4199,26 @@
       </c>
     </row>
     <row r="207" ht="28" spans="3:4">
-      <c r="C207" s="12" t="s">
+      <c r="C207" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D207" s="12" t="s">
+      <c r="D207" s="9" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="208" ht="28" spans="3:4">
-      <c r="C208" s="12" t="s">
+      <c r="C208" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D208" s="12" t="s">
+      <c r="D208" s="9" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="210" ht="56" spans="1:4">
-      <c r="A210" s="10" t="s">
+      <c r="A210" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B210" s="7" t="s">
+      <c r="B210" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C210" s="5" t="s">
@@ -4290,26 +4253,26 @@
       </c>
     </row>
     <row r="214" ht="28" spans="3:4">
-      <c r="C214" s="12" t="s">
+      <c r="C214" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D214" s="12" t="s">
+      <c r="D214" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="215" spans="3:4">
-      <c r="C215" s="12" t="s">
+      <c r="C215" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="D215" s="12" t="s">
+      <c r="D215" s="9" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="217" ht="56" spans="1:4">
-      <c r="A217" s="10" t="s">
+      <c r="A217" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B217" s="7" t="s">
+      <c r="B217" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C217" s="5" t="s">
@@ -4344,26 +4307,26 @@
       </c>
     </row>
     <row r="221" ht="28" spans="3:4">
-      <c r="C221" s="12" t="s">
+      <c r="C221" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D221" s="12" t="s">
+      <c r="D221" s="9" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="222" ht="28" spans="3:4">
-      <c r="C222" s="12" t="s">
+      <c r="C222" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D222" s="12" t="s">
+      <c r="D222" s="9" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="224" ht="42" spans="1:4">
-      <c r="A224" s="10" t="s">
+      <c r="A224" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B224" s="7" t="s">
+      <c r="B224" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C224" s="5" t="s">
@@ -4398,26 +4361,26 @@
       </c>
     </row>
     <row r="228" ht="28" spans="3:4">
-      <c r="C228" s="12" t="s">
+      <c r="C228" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D228" s="12" t="s">
+      <c r="D228" s="9" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="229" spans="3:4">
-      <c r="C229" s="12" t="s">
+      <c r="C229" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D229" s="12" t="s">
+      <c r="D229" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="231" ht="42" spans="1:4">
-      <c r="A231" s="10" t="s">
+      <c r="A231" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B231" s="7" t="s">
+      <c r="B231" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C231" s="5" t="s">
@@ -4452,26 +4415,26 @@
       </c>
     </row>
     <row r="235" ht="28" spans="3:4">
-      <c r="C235" s="12" t="s">
+      <c r="C235" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D235" s="12" t="s">
+      <c r="D235" s="9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="236" spans="3:4">
-      <c r="C236" s="12" t="s">
+      <c r="C236" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="D236" s="12" t="s">
+      <c r="D236" s="9" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="238" ht="56" spans="1:4">
-      <c r="A238" s="10" t="s">
+      <c r="A238" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="7" t="s">
+      <c r="B238" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C238" s="5" t="s">
@@ -4506,26 +4469,26 @@
       </c>
     </row>
     <row r="242" ht="28" spans="3:4">
-      <c r="C242" s="12" t="s">
+      <c r="C242" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="D242" s="12" t="s">
+      <c r="D242" s="9" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="243" ht="28" spans="3:4">
-      <c r="C243" s="12" t="s">
+      <c r="C243" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D243" s="12" t="s">
+      <c r="D243" s="9" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="245" ht="42" spans="1:4">
-      <c r="A245" s="10" t="s">
+      <c r="A245" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B245" s="7" t="s">
+      <c r="B245" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C245" s="5" t="s">
@@ -4560,26 +4523,26 @@
       </c>
     </row>
     <row r="249" ht="28" spans="3:4">
-      <c r="C249" s="12" t="s">
+      <c r="C249" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D249" s="12" t="s">
+      <c r="D249" s="9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="250" spans="3:4">
-      <c r="C250" s="12" t="s">
+      <c r="C250" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="D250" s="12" t="s">
+      <c r="D250" s="9" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="252" ht="42" spans="1:4">
-      <c r="A252" s="10" t="s">
+      <c r="A252" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B252" s="7" t="s">
+      <c r="B252" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C252" s="5" t="s">
@@ -4614,26 +4577,26 @@
       </c>
     </row>
     <row r="256" ht="28" spans="3:4">
-      <c r="C256" s="12" t="s">
+      <c r="C256" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="D256" s="12" t="s">
+      <c r="D256" s="9" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="257" ht="28" spans="3:4">
-      <c r="C257" s="12" t="s">
+      <c r="C257" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D257" s="12" t="s">
+      <c r="D257" s="9" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="259" ht="42" spans="1:4">
-      <c r="A259" s="10" t="s">
+      <c r="A259" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B259" s="7" t="s">
+      <c r="B259" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C259" s="5" t="s">
@@ -4668,26 +4631,26 @@
       </c>
     </row>
     <row r="263" ht="28" spans="3:4">
-      <c r="C263" s="12" t="s">
+      <c r="C263" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D263" s="12" t="s">
+      <c r="D263" s="9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="264" spans="3:4">
-      <c r="C264" s="12" t="s">
+      <c r="C264" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D264" s="12" t="s">
+      <c r="D264" s="9" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="266" ht="42" spans="1:4">
-      <c r="A266" s="10" t="s">
+      <c r="A266" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B266" s="7" t="s">
+      <c r="B266" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C266" s="5" t="s">
@@ -4722,18 +4685,18 @@
       </c>
     </row>
     <row r="270" ht="28" spans="3:4">
-      <c r="C270" s="12" t="s">
+      <c r="C270" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D270" s="12" t="s">
+      <c r="D270" s="9" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="272" ht="42" spans="1:4">
-      <c r="A272" s="10" t="s">
+      <c r="A272" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B272" s="7" t="s">
+      <c r="B272" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C272" s="5" t="s">
@@ -4768,18 +4731,18 @@
       </c>
     </row>
     <row r="276" ht="28" spans="3:4">
-      <c r="C276" s="12" t="s">
+      <c r="C276" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D276" s="12" t="s">
+      <c r="D276" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="278" ht="56" spans="1:4">
-      <c r="A278" s="11" t="s">
+      <c r="A278" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B278" s="7" t="s">
+      <c r="B278" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C278" s="5" t="s">
@@ -4814,34 +4777,34 @@
       </c>
     </row>
     <row r="282" ht="28" spans="3:4">
-      <c r="C282" s="12" t="s">
+      <c r="C282" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D282" s="12" t="s">
+      <c r="D282" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="283" ht="28" spans="3:4">
-      <c r="C283" s="12" t="s">
+      <c r="C283" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="D283" s="12" t="s">
+      <c r="D283" s="9" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="284" spans="3:4">
-      <c r="C284" s="12" t="s">
+      <c r="C284" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="D284" s="12" t="s">
+      <c r="D284" s="9" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="286" ht="56" spans="1:4">
-      <c r="A286" s="11" t="s">
+      <c r="A286" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B286" s="7" t="s">
+      <c r="B286" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C286" s="5" t="s">
@@ -4876,42 +4839,42 @@
       </c>
     </row>
     <row r="290" ht="28" spans="3:4">
-      <c r="C290" s="12" t="s">
+      <c r="C290" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D290" s="12" t="s">
+      <c r="D290" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="291" ht="28" spans="3:4">
-      <c r="C291" s="12" t="s">
+      <c r="C291" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="D291" s="12" t="s">
+      <c r="D291" s="9" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="292" spans="3:4">
-      <c r="C292" s="12" t="s">
+      <c r="C292" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="D292" s="12" t="s">
+      <c r="D292" s="9" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="293" ht="28" spans="3:4">
-      <c r="C293" s="12" t="s">
+      <c r="C293" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D293" s="12" t="s">
+      <c r="D293" s="9" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="295" ht="56" spans="1:4">
-      <c r="A295" s="11" t="s">
+      <c r="A295" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B295" s="7" t="s">
+      <c r="B295" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C295" s="5" t="s">
@@ -4946,26 +4909,26 @@
       </c>
     </row>
     <row r="299" ht="28" spans="3:4">
-      <c r="C299" s="12" t="s">
+      <c r="C299" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D299" s="12" t="s">
+      <c r="D299" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="300" spans="3:4">
-      <c r="C300" s="12" t="s">
+      <c r="C300" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="D300" s="12" t="s">
+      <c r="D300" s="9" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="302" ht="42" spans="1:4">
-      <c r="A302" s="11" t="s">
+      <c r="A302" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B302" s="7" t="s">
+      <c r="B302" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C302" s="5" t="s">
@@ -5000,18 +4963,18 @@
       </c>
     </row>
     <row r="306" ht="28" spans="3:4">
-      <c r="C306" s="12" t="s">
+      <c r="C306" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D306" s="12" t="s">
+      <c r="D306" s="9" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="308" ht="42" spans="1:4">
-      <c r="A308" s="11" t="s">
+      <c r="A308" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B308" s="7" t="s">
+      <c r="B308" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C308" s="5" t="s">
@@ -5046,18 +5009,18 @@
       </c>
     </row>
     <row r="312" spans="3:4">
-      <c r="C312" s="12" t="s">
+      <c r="C312" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D312" s="12" t="s">
+      <c r="D312" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="314" ht="42" spans="1:4">
-      <c r="A314" s="11" t="s">
+      <c r="A314" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B314" s="7" t="s">
+      <c r="B314" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C314" s="5" t="s">
@@ -5092,34 +5055,34 @@
       </c>
     </row>
     <row r="318" spans="3:4">
-      <c r="C318" s="12" t="s">
+      <c r="C318" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D318" s="12" t="s">
+      <c r="D318" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="319" ht="28" spans="3:4">
-      <c r="C319" s="12" t="s">
+      <c r="C319" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D319" s="12" t="s">
+      <c r="D319" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="320" spans="3:4">
-      <c r="C320" s="12" t="s">
+      <c r="C320" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="D320" s="12" t="s">
+      <c r="D320" s="9" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="322" ht="42" spans="1:4">
-      <c r="A322" s="11" t="s">
+      <c r="A322" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B322" s="7" t="s">
+      <c r="B322" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C322" s="5" t="s">
@@ -5154,34 +5117,34 @@
       </c>
     </row>
     <row r="326" spans="3:4">
-      <c r="C326" s="12" t="s">
+      <c r="C326" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D326" s="12" t="s">
+      <c r="D326" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="327" ht="28" spans="3:4">
-      <c r="C327" s="12" t="s">
+      <c r="C327" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D327" s="12" t="s">
+      <c r="D327" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="328" spans="3:4">
-      <c r="C328" s="12" t="s">
+      <c r="C328" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="D328" s="12" t="s">
+      <c r="D328" s="9" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="330" ht="56" spans="1:4">
-      <c r="A330" s="11" t="s">
+      <c r="A330" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B330" s="7" t="s">
+      <c r="B330" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C330" s="5" t="s">
@@ -5216,34 +5179,34 @@
       </c>
     </row>
     <row r="334" spans="3:4">
-      <c r="C334" s="12" t="s">
+      <c r="C334" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D334" s="12" t="s">
+      <c r="D334" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="335" ht="28" spans="3:4">
-      <c r="C335" s="12" t="s">
+      <c r="C335" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D335" s="12" t="s">
+      <c r="D335" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="336" spans="3:4">
-      <c r="C336" s="12" t="s">
+      <c r="C336" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="D336" s="12" t="s">
+      <c r="D336" s="9" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="338" ht="56" spans="1:4">
-      <c r="A338" s="11" t="s">
+      <c r="A338" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B338" s="7" t="s">
+      <c r="B338" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C338" s="5" t="s">
@@ -5278,26 +5241,26 @@
       </c>
     </row>
     <row r="342" ht="28" spans="3:4">
-      <c r="C342" s="12" t="s">
+      <c r="C342" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="D342" s="12" t="s">
+      <c r="D342" s="9" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="343" ht="28" spans="3:4">
-      <c r="C343" s="12" t="s">
+      <c r="C343" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="D343" s="12" t="s">
+      <c r="D343" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="345" ht="56" spans="1:4">
-      <c r="A345" s="11" t="s">
+      <c r="A345" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B345" s="7" t="s">
+      <c r="B345" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C345" s="5" t="s">
@@ -5332,18 +5295,18 @@
       </c>
     </row>
     <row r="349" ht="28" spans="3:4">
-      <c r="C349" s="12" t="s">
+      <c r="C349" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="D349" s="12" t="s">
+      <c r="D349" s="9" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="351" ht="42" spans="1:4">
-      <c r="A351" s="11" t="s">
+      <c r="A351" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B351" s="7" t="s">
+      <c r="B351" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C351" s="5" t="s">
@@ -5378,18 +5341,18 @@
       </c>
     </row>
     <row r="355" ht="28" spans="3:4">
-      <c r="C355" s="12" t="s">
+      <c r="C355" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="D355" s="12" t="s">
+      <c r="D355" s="9" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="357" ht="42" spans="1:4">
-      <c r="A357" s="11" t="s">
+      <c r="A357" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B357" s="7" t="s">
+      <c r="B357" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C357" s="5" t="s">
@@ -5424,18 +5387,18 @@
       </c>
     </row>
     <row r="361" ht="28" spans="3:4">
-      <c r="C361" s="12" t="s">
+      <c r="C361" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="D361" s="12" t="s">
+      <c r="D361" s="9" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="363" ht="42" spans="1:4">
-      <c r="A363" s="11" t="s">
+      <c r="A363" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B363" s="7" t="s">
+      <c r="B363" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C363" s="5" t="s">
@@ -5470,18 +5433,18 @@
       </c>
     </row>
     <row r="367" ht="28" spans="3:4">
-      <c r="C367" s="12" t="s">
+      <c r="C367" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="D367" s="12" t="s">
+      <c r="D367" s="9" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="369" ht="56" spans="1:4">
-      <c r="A369" s="11" t="s">
+      <c r="A369" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B369" s="7" t="s">
+      <c r="B369" s="4" t="s">
         <v>82</v>
       </c>
       <c r="C369" s="5" t="s">
@@ -5492,7 +5455,7 @@
       </c>
     </row>
     <row r="370" spans="2:4">
-      <c r="B370" s="7"/>
+      <c r="B370" s="4"/>
       <c r="C370" s="5" t="s">
         <v>97</v>
       </c>
@@ -5509,7 +5472,7 @@
       </c>
     </row>
     <row r="372" ht="28" spans="2:4">
-      <c r="B372" s="7"/>
+      <c r="B372" s="4"/>
       <c r="C372" s="5" t="s">
         <v>101</v>
       </c>
@@ -5518,18 +5481,18 @@
       </c>
     </row>
     <row r="373" ht="42" spans="3:4">
-      <c r="C373" s="12" t="s">
+      <c r="C373" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="D373" s="12" t="s">
+      <c r="D373" s="9" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="375" ht="70" spans="1:4">
-      <c r="A375" s="11" t="s">
+      <c r="A375" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B375" s="7" t="s">
+      <c r="B375" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C375" s="5" t="s">
@@ -5564,10 +5527,10 @@
       </c>
     </row>
     <row r="379" ht="28" spans="3:4">
-      <c r="C379" s="12" t="s">
+      <c r="C379" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="D379" s="12" t="s">
+      <c r="D379" s="9" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5609,16 +5572,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="19" customHeight="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5626,57 +5589,56 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="10"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="10"/>
-      <c r="C5"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>301</v>
       </c>
     </row>
@@ -5690,7 +5652,7 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -5718,7 +5680,7 @@
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -5762,7 +5724,7 @@
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="3" t="s">
         <v>294</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -6330,8 +6292,8 @@
   <sheetPr/>
   <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
     </sheetView>
@@ -6448,7 +6410,7 @@
       <c r="A7" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>298</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -6518,7 +6480,7 @@
       <c r="A12" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
         <v>300</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -6600,7 +6562,7 @@
       <c r="A18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>301</v>
       </c>
       <c r="C18" s="5" t="s">

</xml_diff>